<commit_message>
basic spreadsheet transformer working
</commit_message>
<xml_diff>
--- a/data/test/excel_2010/excel_2010_test_data.xlsx
+++ b/data/test/excel_2010/excel_2010_test_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
@@ -22,6 +22,9 @@
     <t>givenName</t>
   </si>
   <si>
+    <t>foaf:name</t>
+  </si>
+  <si>
     <t>minor-gordon</t>
   </si>
   <si>
@@ -29,6 +32,9 @@
   </si>
   <si>
     <t>Minor</t>
+  </si>
+  <si>
+    <t>Minor Gordon</t>
   </si>
 </sst>
 </file>
@@ -62,9 +68,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -295,16 +304,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bring SpreadsheetTransformer in line with MarkdownDirectoryTransformer
</commit_message>
<xml_diff>
--- a/data/test/excel_2010/excel_2010_test_data.xlsx
+++ b/data/test/excel_2010/excel_2010_test_data.xlsx
@@ -13,19 +13,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>foaf:familyName</t>
+    <t>@id</t>
+  </si>
+  <si>
+    <t>familyName</t>
   </si>
   <si>
     <t>givenName</t>
   </si>
   <si>
-    <t>foaf:name</t>
-  </si>
-  <si>
-    <t>minor-gordon</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ss-person:minor-gordon</t>
   </si>
   <si>
     <t>Gordon</t>

</xml_diff>

<commit_message>
Excel2010Extractor: handle inserted images
</commit_message>
<xml_diff>
--- a/data/test/excel_2010/excel_2010_test_data.xlsx
+++ b/data/test/excel_2010/excel_2010_test_data.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Person" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Image" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Person" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>depicts</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>ss-person:minor-gordon</t>
+  </si>
   <si>
     <t>@id</t>
   </si>
@@ -23,9 +33,6 @@
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>ss-person:minor-gordon</t>
   </si>
   <si>
     <t>Gordon</t>
@@ -68,13 +75,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -87,6 +95,39 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="295275" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -295,31 +336,60 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating Excel 2010 test data
</commit_message>
<xml_diff>
--- a/data/test/excel_2010/excel_2010_test_data.xlsx
+++ b/data/test/excel_2010/excel_2010_test_data.xlsx
@@ -5,6 +5,8 @@
   <sheets>
     <sheet state="visible" name="Image" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Person" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="WorkCreation" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Work" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>depicts</t>
   </si>
@@ -42,12 +44,33 @@
   </si>
   <si>
     <t>Minor Gordon</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>ss-work:test</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Test work</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -75,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -84,6 +107,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -128,6 +154,14 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -395,4 +429,72 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4">
+        <v>45023.0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update Excel 2010 test data
</commit_message>
<xml_diff>
--- a/data/test/excel_2010/excel_2010_test_data.xlsx
+++ b/data/test/excel_2010/excel_2010_test_data.xlsx
@@ -3,10 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Image" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="DcImage" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="FoafPerson" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="WorkCreation" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Work" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="SchemaCreativeWork" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>@id</t>
   </si>
@@ -46,22 +45,7 @@
     <t>Minor Gordon</t>
   </si>
   <si>
-    <t>creator</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>ss-work-creation:test</t>
-  </si>
-  <si>
-    <t>event</t>
-  </si>
-  <si>
     <t>image</t>
-  </si>
-  <si>
-    <t>title</t>
   </si>
   <si>
     <t>ss-work:test</t>
@@ -74,9 +58,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -104,7 +85,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -113,9 +94,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -164,10 +142,6 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -455,61 +429,18 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4">
-        <v>45023.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new Excel 2010 test data with a stub work
</commit_message>
<xml_diff>
--- a/data/test/excel_2010/excel_2010_test_data.xlsx
+++ b/data/test/excel_2010/excel_2010_test_data.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="DcImage" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="FoafPerson" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="SchemaCreativeWork" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="StubWork" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>@id</t>
   </si>
@@ -48,17 +49,23 @@
     <t>image</t>
   </si>
   <si>
+    <t>#commentheader</t>
+  </si>
+  <si>
     <t>ss-work:test</t>
   </si>
   <si>
     <t>Test work</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q937690</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -69,6 +76,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -94,6 +105,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -142,6 +156,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -431,19 +449,50 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>